<commit_message>
edited IM and EX
</commit_message>
<xml_diff>
--- a/data/Monthly Mastersheet with Original Data.xlsx
+++ b/data/Monthly Mastersheet with Original Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianyishen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliceye/Desktop/CryptoMacroecon-Prediction-CSUREMM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8497636-AB20-F741-9329-A5881C7251CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC51D38-3CB0-6B4A-A2F1-C9EC0BB5CE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="2640" windowWidth="29400" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="25420" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6.30 data" sheetId="3" r:id="rId1"/>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1120,11 +1120,11 @@
       <c r="M2" s="5">
         <v>3535.6</v>
       </c>
-      <c r="N2" s="5">
-        <v>2916.0219999999999</v>
-      </c>
-      <c r="O2" s="5">
-        <v>2535.5010000000002</v>
+      <c r="N2" s="24">
+        <v>193973.8694</v>
+      </c>
+      <c r="O2">
+        <v>201125</v>
       </c>
       <c r="P2" s="5">
         <v>95.1</v>
@@ -1169,11 +1169,11 @@
       <c r="M3" s="5">
         <v>3615</v>
       </c>
-      <c r="N3" s="5">
-        <v>3034.0039999999999</v>
-      </c>
-      <c r="O3" s="5">
-        <v>2479.107</v>
+      <c r="N3" s="24">
+        <v>196998.9161</v>
+      </c>
+      <c r="O3">
+        <v>202855</v>
       </c>
       <c r="P3" s="5">
         <v>100.7</v>
@@ -1218,11 +1218,11 @@
       <c r="M4" s="5">
         <v>3587.6</v>
       </c>
-      <c r="N4" s="5">
-        <v>3034.0039999999999</v>
-      </c>
-      <c r="O4" s="5">
-        <v>2479.107</v>
+      <c r="N4" s="24">
+        <v>203634.48199999999</v>
+      </c>
+      <c r="O4">
+        <v>206890</v>
       </c>
       <c r="P4" s="5">
         <v>98.5</v>
@@ -1267,11 +1267,11 @@
       <c r="M5" s="5">
         <v>3630.5</v>
       </c>
-      <c r="N5" s="5">
-        <v>3034.0039999999999</v>
-      </c>
-      <c r="O5" s="5">
-        <v>2479.107</v>
+      <c r="N5" s="24">
+        <v>207891.54930000001</v>
+      </c>
+      <c r="O5">
+        <v>209690</v>
       </c>
       <c r="P5" s="5">
         <v>95.9</v>
@@ -1316,11 +1316,11 @@
       <c r="M6" s="5">
         <v>3673.4</v>
       </c>
-      <c r="N6" s="5">
-        <v>3093.299</v>
-      </c>
-      <c r="O6" s="5">
-        <v>2517.268</v>
+      <c r="N6" s="24">
+        <v>206553.2303</v>
+      </c>
+      <c r="O6">
+        <v>207358</v>
       </c>
       <c r="P6" s="5">
         <v>95.7</v>
@@ -1367,11 +1367,11 @@
       <c r="M7" s="5">
         <v>3568.2</v>
       </c>
-      <c r="N7" s="5">
-        <v>3093.299</v>
-      </c>
-      <c r="O7" s="5">
-        <v>2517.268</v>
+      <c r="N7" s="24">
+        <v>210566.1318</v>
+      </c>
+      <c r="O7">
+        <v>210539</v>
       </c>
       <c r="P7" s="5">
         <v>99.7</v>
@@ -1418,11 +1418,11 @@
       <c r="M8" s="5">
         <v>3655.7</v>
       </c>
-      <c r="N8" s="5">
-        <v>3093.299</v>
-      </c>
-      <c r="O8" s="5">
-        <v>2517.268</v>
+      <c r="N8" s="24">
+        <v>208532.82490000001</v>
+      </c>
+      <c r="O8">
+        <v>213280</v>
       </c>
       <c r="P8" s="5">
         <v>101.4</v>
@@ -1469,11 +1469,11 @@
       <c r="M9" s="5">
         <v>3728.7</v>
       </c>
-      <c r="N9" s="5">
-        <v>3105.9949999999999</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2562.172</v>
+      <c r="N9" s="24">
+        <v>209993.3964</v>
+      </c>
+      <c r="O9">
+        <v>212156</v>
       </c>
       <c r="P9" s="5">
         <v>98.8</v>
@@ -1520,11 +1520,11 @@
       <c r="M10" s="5">
         <v>3632.5</v>
       </c>
-      <c r="N10" s="5">
-        <v>3105.9949999999999</v>
-      </c>
-      <c r="O10" s="5">
-        <v>2562.172</v>
+      <c r="N10" s="24">
+        <v>208636.6458</v>
+      </c>
+      <c r="O10">
+        <v>215578</v>
       </c>
       <c r="P10" s="5">
         <v>98</v>
@@ -1571,11 +1571,11 @@
       <c r="M11" s="5">
         <v>3645.5</v>
       </c>
-      <c r="N11" s="5">
-        <v>3105.9949999999999</v>
-      </c>
-      <c r="O11" s="5">
-        <v>2562.172</v>
+      <c r="N11" s="24">
+        <v>209572.02720000001</v>
+      </c>
+      <c r="O11">
+        <v>213466</v>
       </c>
       <c r="P11" s="5">
         <v>98.2</v>
@@ -1622,11 +1622,11 @@
       <c r="M12" s="5">
         <v>3699.4</v>
       </c>
-      <c r="N12" s="5">
-        <v>3153.7469999999998</v>
-      </c>
-      <c r="O12" s="5">
-        <v>2535.5010000000002</v>
+      <c r="N12" s="24">
+        <v>212417.06080000001</v>
+      </c>
+      <c r="O12">
+        <v>211540</v>
       </c>
       <c r="P12" s="5">
         <v>97.9</v>
@@ -1673,11 +1673,11 @@
       <c r="M13" s="5">
         <v>3664.8</v>
       </c>
-      <c r="N13" s="5">
-        <v>3153.7469999999998</v>
-      </c>
-      <c r="O13" s="5">
-        <v>2535.5010000000002</v>
+      <c r="N13" s="24">
+        <v>212257.98209999999</v>
+      </c>
+      <c r="O13">
+        <v>211420</v>
       </c>
       <c r="P13" s="5">
         <v>96.2</v>
@@ -1724,11 +1724,11 @@
       <c r="M14" s="5">
         <v>3678.4</v>
       </c>
-      <c r="N14" s="5">
-        <v>3153.7469999999998</v>
-      </c>
-      <c r="O14" s="5">
-        <v>2535.5010000000002</v>
+      <c r="N14" s="24">
+        <v>215409.59460000001</v>
+      </c>
+      <c r="O14">
+        <v>213852</v>
       </c>
       <c r="P14" s="5">
         <v>100.1</v>
@@ -1775,11 +1775,11 @@
       <c r="M15" s="5">
         <v>3727.4</v>
       </c>
-      <c r="N15" s="5">
-        <v>3171.6219999999998</v>
-      </c>
-      <c r="O15" s="5">
-        <v>2537.415</v>
+      <c r="N15" s="24">
+        <v>217026.4149</v>
+      </c>
+      <c r="O15">
+        <v>214288</v>
       </c>
       <c r="P15" s="5">
         <v>98.6</v>
@@ -1826,11 +1826,11 @@
       <c r="M16" s="5">
         <v>3664.2</v>
       </c>
-      <c r="N16" s="5">
-        <v>3171.6219999999998</v>
-      </c>
-      <c r="O16" s="5">
-        <v>2537.415</v>
+      <c r="N16" s="24">
+        <v>210969.72649999999</v>
+      </c>
+      <c r="O16">
+        <v>211755</v>
       </c>
       <c r="P16" s="5">
         <v>97.5</v>
@@ -1877,11 +1877,11 @@
       <c r="M17" s="5">
         <v>3814.2</v>
       </c>
-      <c r="N17" s="5">
-        <v>3171.6219999999998</v>
-      </c>
-      <c r="O17" s="5">
-        <v>2537.415</v>
+      <c r="N17" s="24">
+        <v>214210.2384</v>
+      </c>
+      <c r="O17">
+        <v>209350</v>
       </c>
       <c r="P17" s="5">
         <v>98.3</v>
@@ -1930,11 +1930,11 @@
       <c r="M18" s="5">
         <v>3728.9</v>
       </c>
-      <c r="N18" s="5">
-        <v>3132.5390000000002</v>
-      </c>
-      <c r="O18" s="5">
-        <v>2540.2440000000001</v>
+      <c r="N18" s="24">
+        <v>209025.2537</v>
+      </c>
+      <c r="O18">
+        <v>211144</v>
       </c>
       <c r="P18" s="5">
         <v>91.2</v>
@@ -1983,11 +1983,11 @@
       <c r="M19" s="5">
         <v>3710.7</v>
       </c>
-      <c r="N19" s="5">
-        <v>3132.5390000000002</v>
-      </c>
-      <c r="O19" s="5">
-        <v>2540.2440000000001</v>
+      <c r="N19" s="24">
+        <v>209281.38219999999</v>
+      </c>
+      <c r="O19">
+        <v>213288</v>
       </c>
       <c r="P19" s="5">
         <v>93.8</v>
@@ -2036,11 +2036,11 @@
       <c r="M20" s="5">
         <v>3726.1</v>
       </c>
-      <c r="N20" s="5">
-        <v>3132.5390000000002</v>
-      </c>
-      <c r="O20" s="5">
-        <v>2540.2440000000001</v>
+      <c r="N20" s="24">
+        <v>210780.74770000001</v>
+      </c>
+      <c r="O20">
+        <v>214650</v>
       </c>
       <c r="P20" s="5">
         <v>98.4</v>
@@ -2089,11 +2089,11 @@
       <c r="M21" s="5">
         <v>3843.9</v>
       </c>
-      <c r="N21" s="5">
-        <v>3165.41</v>
-      </c>
-      <c r="O21" s="5">
-        <v>2547.4479999999999</v>
+      <c r="N21" s="24">
+        <v>208800.1727</v>
+      </c>
+      <c r="O21">
+        <v>211246</v>
       </c>
       <c r="P21" s="5">
         <v>97.2</v>
@@ -2142,11 +2142,11 @@
       <c r="M22" s="5">
         <v>3761</v>
       </c>
-      <c r="N22" s="5">
-        <v>3165.41</v>
-      </c>
-      <c r="O22" s="5">
-        <v>2547.4479999999999</v>
+      <c r="N22" s="24">
+        <v>214094.93049999999</v>
+      </c>
+      <c r="O22">
+        <v>215480</v>
       </c>
       <c r="P22" s="5">
         <v>100</v>
@@ -2195,11 +2195,11 @@
       <c r="M23" s="5">
         <v>3825.2</v>
       </c>
-      <c r="N23" s="5">
-        <v>3165.41</v>
-      </c>
-      <c r="O23" s="5">
-        <v>2547.4479999999999</v>
+      <c r="N23" s="24">
+        <v>209355.7169</v>
+      </c>
+      <c r="O23">
+        <v>212818</v>
       </c>
       <c r="P23" s="5">
         <v>98.2</v>
@@ -2248,11 +2248,11 @@
       <c r="M24" s="5">
         <v>3872.9</v>
       </c>
-      <c r="N24" s="5">
-        <v>3117.9520000000002</v>
-      </c>
-      <c r="O24" s="5">
-        <v>2532.4050000000002</v>
+      <c r="N24" s="24">
+        <v>209386.8118</v>
+      </c>
+      <c r="O24">
+        <v>212797</v>
       </c>
       <c r="P24" s="5">
         <v>98.4</v>
@@ -2301,11 +2301,11 @@
       <c r="M25" s="5">
         <v>3833.5</v>
       </c>
-      <c r="N25" s="5">
-        <v>3117.9520000000002</v>
-      </c>
-      <c r="O25" s="5">
-        <v>2532.4050000000002</v>
+      <c r="N25" s="24">
+        <v>209358.0675</v>
+      </c>
+      <c r="O25">
+        <v>212599</v>
       </c>
       <c r="P25" s="5">
         <v>89.8</v>
@@ -2354,11 +2354,11 @@
       <c r="M26" s="5">
         <v>3903.1</v>
       </c>
-      <c r="N26" s="5">
-        <v>3117.9520000000002</v>
-      </c>
-      <c r="O26" s="5">
-        <v>2532.4050000000002</v>
+      <c r="N26" s="24">
+        <v>204455.6306</v>
+      </c>
+      <c r="O26">
+        <v>211602</v>
       </c>
       <c r="P26" s="5">
         <v>93.2</v>
@@ -2407,11 +2407,11 @@
       <c r="M27" s="5">
         <v>3898.3</v>
       </c>
-      <c r="N27" s="5">
-        <v>3050.8240000000001</v>
-      </c>
-      <c r="O27" s="5">
-        <v>2537.4659999999999</v>
+      <c r="N27" s="24">
+        <v>202068.37160000001</v>
+      </c>
+      <c r="O27">
+        <v>212281</v>
       </c>
       <c r="P27" s="5">
         <v>95.5</v>
@@ -2460,11 +2460,11 @@
       <c r="M28" s="5">
         <v>3916.2</v>
       </c>
-      <c r="N28" s="5">
-        <v>3050.8240000000001</v>
-      </c>
-      <c r="O28" s="5">
-        <v>2537.4659999999999</v>
+      <c r="N28" s="24">
+        <v>200193.467</v>
+      </c>
+      <c r="O28">
+        <v>212786</v>
       </c>
       <c r="P28" s="5">
         <v>96.8</v>
@@ -2513,11 +2513,11 @@
       <c r="M29" s="5">
         <v>4051.6</v>
       </c>
-      <c r="N29" s="5">
-        <v>3050.8240000000001</v>
-      </c>
-      <c r="O29" s="5">
-        <v>2537.4659999999999</v>
+      <c r="N29" s="24">
+        <v>204899.01550000001</v>
+      </c>
+      <c r="O29">
+        <v>213402</v>
       </c>
       <c r="P29" s="5">
         <v>99.3</v>
@@ -2566,11 +2566,11 @@
       <c r="M30" s="5">
         <v>3960.6</v>
       </c>
-      <c r="N30" s="5">
-        <v>2929.759</v>
-      </c>
-      <c r="O30" s="5">
-        <v>2416.181</v>
+      <c r="N30" s="24">
+        <v>201885.35190000001</v>
+      </c>
+      <c r="O30">
+        <v>208878</v>
       </c>
       <c r="P30" s="5">
         <v>99.8</v>
@@ -2619,11 +2619,11 @@
       <c r="M31" s="5">
         <v>3950.5</v>
       </c>
-      <c r="N31" s="5">
-        <v>2929.759</v>
-      </c>
-      <c r="O31" s="5">
-        <v>2416.181</v>
+      <c r="N31" s="24">
+        <v>198128.56210000001</v>
+      </c>
+      <c r="O31">
+        <v>209544</v>
       </c>
       <c r="P31" s="5">
         <v>101</v>
@@ -2672,11 +2672,11 @@
       <c r="M32" s="5">
         <v>4244.2</v>
       </c>
-      <c r="N32" s="5">
-        <v>2929.759</v>
-      </c>
-      <c r="O32" s="5">
-        <v>2416.181</v>
+      <c r="N32" s="24">
+        <v>190862.69380000001</v>
+      </c>
+      <c r="O32">
+        <v>190055</v>
       </c>
       <c r="P32" s="5">
         <v>89.1</v>
@@ -2725,11 +2725,11 @@
       <c r="M33" s="5">
         <v>4804</v>
       </c>
-      <c r="N33" s="5">
-        <v>2350.9259999999999</v>
-      </c>
-      <c r="O33" s="5">
-        <v>1814.4010000000001</v>
+      <c r="N33" s="24">
+        <v>168318.23069999999</v>
+      </c>
+      <c r="O33">
+        <v>151929</v>
       </c>
       <c r="P33" s="5">
         <v>71.8</v>
@@ -2778,11 +2778,11 @@
       <c r="M34" s="5">
         <v>16100.1</v>
       </c>
-      <c r="N34" s="5">
-        <v>2350.9259999999999</v>
-      </c>
-      <c r="O34" s="5">
-        <v>1814.4010000000001</v>
+      <c r="N34" s="24">
+        <v>166040.92079999999</v>
+      </c>
+      <c r="O34">
+        <v>147143</v>
       </c>
       <c r="P34" s="5">
         <v>72.3</v>
@@ -2831,11 +2831,11 @@
       <c r="M35" s="5">
         <v>16496</v>
       </c>
-      <c r="N35" s="5">
-        <v>2350.9259999999999</v>
-      </c>
-      <c r="O35" s="5">
-        <v>1814.4010000000001</v>
+      <c r="N35" s="24">
+        <v>174324.6329</v>
+      </c>
+      <c r="O35">
+        <v>160760</v>
       </c>
       <c r="P35" s="5">
         <v>78.099999999999994</v>
@@ -2884,11 +2884,11 @@
       <c r="M36" s="5">
         <v>16745.3</v>
       </c>
-      <c r="N36" s="5">
-        <v>2801.482</v>
-      </c>
-      <c r="O36" s="5">
-        <v>2105.0830000000001</v>
+      <c r="N36" s="24">
+        <v>194876.10209999999</v>
+      </c>
+      <c r="O36">
+        <v>172697</v>
       </c>
       <c r="P36" s="5">
         <v>72.5</v>
@@ -2937,11 +2937,11 @@
       <c r="M37" s="5">
         <v>16846.8</v>
       </c>
-      <c r="N37" s="5">
-        <v>2801.482</v>
-      </c>
-      <c r="O37" s="5">
-        <v>2105.0830000000001</v>
+      <c r="N37" s="24">
+        <v>200956.0012</v>
+      </c>
+      <c r="O37">
+        <v>176731</v>
       </c>
       <c r="P37" s="5">
         <v>74.099999999999994</v>
@@ -2990,11 +2990,11 @@
       <c r="M38" s="5">
         <v>17128.5</v>
       </c>
-      <c r="N38" s="5">
-        <v>2801.482</v>
-      </c>
-      <c r="O38" s="5">
-        <v>2105.0830000000001</v>
+      <c r="N38" s="24">
+        <v>200321.20980000001</v>
+      </c>
+      <c r="O38">
+        <v>182527</v>
       </c>
       <c r="P38" s="5">
         <v>80.400000000000006</v>
@@ -3043,11 +3043,11 @@
       <c r="M39" s="5">
         <v>17280.7</v>
       </c>
-      <c r="N39" s="5">
-        <v>3027.1990000000001</v>
-      </c>
-      <c r="O39" s="5">
-        <v>2268.8910000000001</v>
+      <c r="N39" s="24">
+        <v>206545.0485</v>
+      </c>
+      <c r="O39">
+        <v>185902</v>
       </c>
       <c r="P39" s="5">
         <v>81.8</v>
@@ -3096,11 +3096,11 @@
       <c r="M40" s="5">
         <v>17604</v>
       </c>
-      <c r="N40" s="5">
-        <v>3027.1990000000001</v>
-      </c>
-      <c r="O40" s="5">
-        <v>2268.8910000000001</v>
+      <c r="N40" s="24">
+        <v>213303.23920000001</v>
+      </c>
+      <c r="O40">
+        <v>190228</v>
       </c>
       <c r="P40" s="5">
         <v>76.900000000000006</v>
@@ -3149,11 +3149,11 @@
       <c r="M41" s="5">
         <v>17920.099999999999</v>
       </c>
-      <c r="N41" s="5">
-        <v>3027.1990000000001</v>
-      </c>
-      <c r="O41" s="5">
-        <v>2268.8910000000001</v>
+      <c r="N41" s="24">
+        <v>215915.18770000001</v>
+      </c>
+      <c r="O41">
+        <v>196454</v>
       </c>
       <c r="P41" s="5">
         <v>80.7</v>
@@ -3202,11 +3202,11 @@
       <c r="M42" s="5">
         <v>18064.5</v>
       </c>
-      <c r="N42" s="5">
-        <v>3176.982</v>
-      </c>
-      <c r="O42" s="5">
-        <v>2381.2240000000002</v>
+      <c r="N42" s="24">
+        <v>219282.94200000001</v>
+      </c>
+      <c r="O42">
+        <v>199093</v>
       </c>
       <c r="P42" s="5">
         <v>79</v>
@@ -3255,11 +3255,11 @@
       <c r="M43" s="5">
         <v>18185.5</v>
       </c>
-      <c r="N43" s="5">
-        <v>3176.982</v>
-      </c>
-      <c r="O43" s="5">
-        <v>2381.2240000000002</v>
+      <c r="N43" s="24">
+        <v>218351.0056</v>
+      </c>
+      <c r="O43">
+        <v>195739</v>
       </c>
       <c r="P43" s="5">
         <v>76.8</v>
@@ -3308,11 +3308,11 @@
       <c r="M44" s="5">
         <v>18622.599999999999</v>
       </c>
-      <c r="N44" s="5">
-        <v>3176.982</v>
-      </c>
-      <c r="O44" s="5">
-        <v>2381.2240000000002</v>
+      <c r="N44" s="24">
+        <v>230164.4987</v>
+      </c>
+      <c r="O44">
+        <v>208951</v>
       </c>
       <c r="P44" s="5">
         <v>84.9</v>
@@ -3361,11 +3361,11 @@
       <c r="M45" s="5">
         <v>19052.099999999999</v>
       </c>
-      <c r="N45" s="5">
-        <v>3340.114</v>
-      </c>
-      <c r="O45" s="5">
-        <v>2505.0320000000002</v>
+      <c r="N45" s="24">
+        <v>228751.63819999999</v>
+      </c>
+      <c r="O45">
+        <v>209117</v>
       </c>
       <c r="P45" s="5">
         <v>88.3</v>
@@ -3414,11 +3414,11 @@
       <c r="M46" s="5">
         <v>19127.099999999999</v>
       </c>
-      <c r="N46" s="5">
-        <v>3340.114</v>
-      </c>
-      <c r="O46" s="5">
-        <v>2505.0320000000002</v>
+      <c r="N46" s="24">
+        <v>230774.98149999999</v>
+      </c>
+      <c r="O46">
+        <v>211641</v>
       </c>
       <c r="P46" s="5">
         <v>82.9</v>
@@ -3467,11 +3467,11 @@
       <c r="M47" s="5">
         <v>19264.900000000001</v>
       </c>
-      <c r="N47" s="5">
-        <v>3340.114</v>
-      </c>
-      <c r="O47" s="5">
-        <v>2505.0320000000002</v>
+      <c r="N47" s="24">
+        <v>236397.0447</v>
+      </c>
+      <c r="O47">
+        <v>214009</v>
       </c>
       <c r="P47" s="5">
         <v>85.5</v>
@@ -3520,11 +3520,11 @@
       <c r="M48" s="5">
         <v>19425.7</v>
       </c>
-      <c r="N48" s="5">
-        <v>3458.7829999999999</v>
-      </c>
-      <c r="O48" s="5">
-        <v>2570.1030000000001</v>
+      <c r="N48" s="24">
+        <v>233642.1581</v>
+      </c>
+      <c r="O48">
+        <v>216286</v>
       </c>
       <c r="P48" s="5">
         <v>81.2</v>
@@ -3573,11 +3573,11 @@
       <c r="M49" s="5">
         <v>19635</v>
       </c>
-      <c r="N49" s="5">
-        <v>3458.7829999999999</v>
-      </c>
-      <c r="O49" s="5">
-        <v>2570.1030000000001</v>
+      <c r="N49" s="24">
+        <v>236969.89730000001</v>
+      </c>
+      <c r="O49">
+        <v>217728</v>
       </c>
       <c r="P49" s="5">
         <v>70.3</v>
@@ -3626,11 +3626,11 @@
       <c r="M50" s="5">
         <v>19827.599999999999</v>
       </c>
-      <c r="N50" s="5">
-        <v>3458.7829999999999</v>
-      </c>
-      <c r="O50" s="5">
-        <v>2570.1030000000001</v>
+      <c r="N50" s="24">
+        <v>236556.95970000001</v>
+      </c>
+      <c r="O50">
+        <v>214183</v>
       </c>
       <c r="P50" s="5">
         <v>72.8</v>
@@ -3679,11 +3679,11 @@
       <c r="M51" s="5">
         <v>19988.3</v>
       </c>
-      <c r="N51" s="5">
-        <v>3685.9560000000001</v>
-      </c>
-      <c r="O51" s="5">
-        <v>2765.36</v>
+      <c r="N51" s="24">
+        <v>241691.77429999999</v>
+      </c>
+      <c r="O51">
+        <v>228772</v>
       </c>
       <c r="P51" s="5">
         <v>71.7</v>
@@ -3732,11 +3732,11 @@
       <c r="M52" s="5">
         <v>20225</v>
       </c>
-      <c r="N52" s="5">
-        <v>3685.9560000000001</v>
-      </c>
-      <c r="O52" s="5">
-        <v>2765.36</v>
+      <c r="N52" s="24">
+        <v>255960.21280000001</v>
+      </c>
+      <c r="O52">
+        <v>231756</v>
       </c>
       <c r="P52" s="5">
         <v>67.400000000000006</v>
@@ -3785,11 +3785,11 @@
       <c r="M53" s="5">
         <v>20567.900000000001</v>
       </c>
-      <c r="N53" s="5">
-        <v>3685.9560000000001</v>
-      </c>
-      <c r="O53" s="5">
-        <v>2765.36</v>
+      <c r="N53" s="24">
+        <v>259972.38709999999</v>
+      </c>
+      <c r="O53">
+        <v>236793</v>
       </c>
       <c r="P53" s="5">
         <v>70.599999999999994</v>
@@ -3838,11 +3838,11 @@
       <c r="M54" s="5">
         <v>20555.5</v>
       </c>
-      <c r="N54" s="5">
-        <v>3925.7420000000002</v>
-      </c>
-      <c r="O54" s="5">
-        <v>2848.6979999999999</v>
+      <c r="N54" s="24">
+        <v>261133.77069999999</v>
+      </c>
+      <c r="O54">
+        <v>232637</v>
       </c>
       <c r="P54" s="5">
         <v>67.2</v>
@@ -3891,11 +3891,11 @@
       <c r="M55" s="5">
         <v>20523.599999999999</v>
       </c>
-      <c r="N55" s="5">
-        <v>3925.7420000000002</v>
-      </c>
-      <c r="O55" s="5">
-        <v>2848.6979999999999</v>
+      <c r="N55" s="24">
+        <v>263790.00599999999</v>
+      </c>
+      <c r="O55">
+        <v>237005</v>
       </c>
       <c r="P55" s="5">
         <v>62.8</v>
@@ -3944,11 +3944,11 @@
       <c r="M56" s="5">
         <v>20789.400000000001</v>
       </c>
-      <c r="N56" s="5">
-        <v>3925.7420000000002</v>
-      </c>
-      <c r="O56" s="5">
-        <v>2848.6979999999999</v>
+      <c r="N56" s="24">
+        <v>288926.6066</v>
+      </c>
+      <c r="O56">
+        <v>248299</v>
       </c>
       <c r="P56" s="5">
         <v>59.4</v>
@@ -3997,11 +3997,11 @@
       <c r="M57" s="5">
         <v>20873.400000000001</v>
       </c>
-      <c r="N57" s="5">
-        <v>4093.663</v>
-      </c>
-      <c r="O57" s="5">
-        <v>3071.5509999999999</v>
+      <c r="N57" s="24">
+        <v>279054.9743</v>
+      </c>
+      <c r="O57">
+        <v>256715</v>
       </c>
       <c r="P57" s="5">
         <v>65.2</v>
@@ -4050,11 +4050,11 @@
       <c r="M58" s="5">
         <v>20552.900000000001</v>
       </c>
-      <c r="N58" s="5">
-        <v>4093.663</v>
-      </c>
-      <c r="O58" s="5">
-        <v>3071.5509999999999</v>
+      <c r="N58" s="24">
+        <v>279341.61379999999</v>
+      </c>
+      <c r="O58">
+        <v>259050</v>
       </c>
       <c r="P58" s="5">
         <v>58.4</v>
@@ -4103,11 +4103,11 @@
       <c r="M59" s="5">
         <v>20542.3</v>
       </c>
-      <c r="N59" s="5">
-        <v>4093.663</v>
-      </c>
-      <c r="O59" s="5">
-        <v>3071.5509999999999</v>
+      <c r="N59" s="24">
+        <v>279308.28739999997</v>
+      </c>
+      <c r="O59">
+        <v>262615</v>
       </c>
       <c r="P59" s="5">
         <v>50</v>
@@ -4156,11 +4156,11 @@
       <c r="M60" s="5">
         <v>20492.2</v>
       </c>
-      <c r="N60" s="5">
-        <v>3988.4470000000001</v>
-      </c>
-      <c r="O60" s="5">
-        <v>3102.55</v>
+      <c r="N60" s="24">
+        <v>269553.28600000002</v>
+      </c>
+      <c r="O60">
+        <v>265032</v>
       </c>
       <c r="P60" s="5">
         <v>51.5</v>
@@ -4209,11 +4209,11 @@
       <c r="M61" s="5">
         <v>20411.2</v>
       </c>
-      <c r="N61" s="5">
-        <v>3988.4470000000001</v>
-      </c>
-      <c r="O61" s="5">
-        <v>3102.55</v>
+      <c r="N61" s="24">
+        <v>268103.33480000001</v>
+      </c>
+      <c r="O61">
+        <v>265216</v>
       </c>
       <c r="P61" s="5">
         <v>58.2</v>
@@ -4262,11 +4262,11 @@
       <c r="M62" s="5">
         <v>20265.400000000001</v>
       </c>
-      <c r="N62" s="5">
-        <v>3988.4470000000001</v>
-      </c>
-      <c r="O62" s="5">
-        <v>3102.55</v>
+      <c r="N62" s="24">
+        <v>265814.63740000001</v>
+      </c>
+      <c r="O62">
+        <v>262473</v>
       </c>
       <c r="P62" s="5">
         <v>58.6</v>
@@ -4315,11 +4315,11 @@
       <c r="M63" s="5">
         <v>20063.400000000001</v>
       </c>
-      <c r="N63" s="5">
-        <v>3897.402</v>
-      </c>
-      <c r="O63" s="5">
-        <v>3046.7179999999998</v>
+      <c r="N63" s="24">
+        <v>270299.08860000002</v>
+      </c>
+      <c r="O63">
+        <v>259671</v>
       </c>
       <c r="P63" s="5">
         <v>59.9</v>
@@ -4368,11 +4368,11 @@
       <c r="M64" s="5">
         <v>19943.900000000001</v>
       </c>
-      <c r="N64" s="5">
-        <v>3897.402</v>
-      </c>
-      <c r="O64" s="5">
-        <v>3046.7179999999998</v>
+      <c r="N64" s="24">
+        <v>254661.8573</v>
+      </c>
+      <c r="O64">
+        <v>256225</v>
       </c>
       <c r="P64" s="5">
         <v>56.7</v>
@@ -4421,11 +4421,11 @@
       <c r="M65" s="5">
         <v>19871.2</v>
       </c>
-      <c r="N65" s="5">
-        <v>3897.402</v>
-      </c>
-      <c r="O65" s="5">
-        <v>3046.7179999999998</v>
+      <c r="N65" s="24">
+        <v>259745.4718</v>
+      </c>
+      <c r="O65">
+        <v>253508</v>
       </c>
       <c r="P65" s="5">
         <v>59.8</v>
@@ -4474,11 +4474,11 @@
       <c r="M66" s="5">
         <v>19582.3</v>
       </c>
-      <c r="N66" s="5">
-        <v>3874.21</v>
-      </c>
-      <c r="O66" s="5">
-        <v>3060.5619999999999</v>
+      <c r="N66" s="24">
+        <v>264143.55739999999</v>
+      </c>
+      <c r="O66">
+        <v>259974</v>
       </c>
       <c r="P66" s="5">
         <v>64.900000000000006</v>
@@ -4527,11 +4527,11 @@
       <c r="M67" s="5">
         <v>19285.8</v>
       </c>
-      <c r="N67" s="5">
-        <v>3874.21</v>
-      </c>
-      <c r="O67" s="5">
-        <v>3060.5619999999999</v>
+      <c r="N67" s="24">
+        <v>258962.17259999999</v>
+      </c>
+      <c r="O67">
+        <v>254337</v>
       </c>
       <c r="P67" s="5">
         <v>66.900000000000006</v>
@@ -4580,11 +4580,11 @@
       <c r="M68" s="5">
         <v>19072.099999999999</v>
       </c>
-      <c r="N68" s="5">
-        <v>3874.21</v>
-      </c>
-      <c r="O68" s="5">
-        <v>3060.5619999999999</v>
+      <c r="N68" s="24">
+        <v>253489.45319999999</v>
+      </c>
+      <c r="O68">
+        <v>259541</v>
       </c>
       <c r="P68" s="5">
         <v>62</v>
@@ -4633,11 +4633,11 @@
       <c r="M69" s="5">
         <v>18777</v>
       </c>
-      <c r="N69" s="5">
-        <v>3799.0030000000002</v>
-      </c>
-      <c r="O69" s="5">
-        <v>2995.5239999999999</v>
+      <c r="N69" s="24">
+        <v>259147.38959999999</v>
+      </c>
+      <c r="O69">
+        <v>253608</v>
       </c>
       <c r="P69" s="5">
         <v>63.7</v>
@@ -4686,11 +4686,11 @@
       <c r="M70" s="5">
         <v>18450.2</v>
       </c>
-      <c r="N70" s="5">
-        <v>3799.0030000000002</v>
-      </c>
-      <c r="O70" s="5">
-        <v>2995.5239999999999</v>
+      <c r="N70" s="24">
+        <v>253230.8554</v>
+      </c>
+      <c r="O70">
+        <v>252569</v>
       </c>
       <c r="P70" s="5">
         <v>59</v>
@@ -4739,11 +4739,11 @@
       <c r="M71" s="5">
         <v>18403.599999999999</v>
       </c>
-      <c r="N71" s="5">
-        <v>3799.0030000000002</v>
-      </c>
-      <c r="O71" s="5">
-        <v>2995.5239999999999</v>
+      <c r="N71" s="24">
+        <v>251577.24350000001</v>
+      </c>
+      <c r="O71">
+        <v>251879</v>
       </c>
       <c r="P71" s="5">
         <v>64.2</v>
@@ -4792,11 +4792,11 @@
       <c r="M72" s="5">
         <v>18303.400000000001</v>
       </c>
-      <c r="N72" s="5">
-        <v>3843.1320000000001</v>
-      </c>
-      <c r="O72" s="5">
-        <v>3062.0410000000002</v>
+      <c r="N72" s="24">
+        <v>254490.58429999999</v>
+      </c>
+      <c r="O72">
+        <v>255576</v>
       </c>
       <c r="P72" s="5">
         <v>71.5</v>
@@ -4845,11 +4845,11 @@
       <c r="M73" s="5">
         <v>18187.8</v>
       </c>
-      <c r="N73" s="5">
-        <v>3843.1320000000001</v>
-      </c>
-      <c r="O73" s="5">
-        <v>3062.0410000000002</v>
+      <c r="N73" s="24">
+        <v>253943.32560000001</v>
+      </c>
+      <c r="O73">
+        <v>259963</v>
       </c>
       <c r="P73" s="5">
         <v>69.400000000000006</v>
@@ -4898,11 +4898,11 @@
       <c r="M74" s="5">
         <v>18104.2</v>
       </c>
-      <c r="N74" s="5">
-        <v>3843.1320000000001</v>
-      </c>
-      <c r="O74" s="5">
-        <v>3062.0410000000002</v>
+      <c r="N74" s="24">
+        <v>256709.57329999999</v>
+      </c>
+      <c r="O74">
+        <v>263533</v>
       </c>
       <c r="P74" s="5">
         <v>67.8</v>
@@ -4951,11 +4951,11 @@
       <c r="M75" s="5">
         <v>17992</v>
       </c>
-      <c r="N75" s="5">
-        <v>3882.8989999999999</v>
-      </c>
-      <c r="O75" s="5">
-        <v>3091.748</v>
+      <c r="N75" s="24">
+        <v>259092.01869999999</v>
+      </c>
+      <c r="O75">
+        <v>262463</v>
       </c>
       <c r="P75" s="5">
         <v>63.8</v>
@@ -5004,11 +5004,11 @@
       <c r="M76" s="5">
         <v>17964.8</v>
       </c>
-      <c r="N76" s="5">
-        <v>3882.8989999999999</v>
-      </c>
-      <c r="O76" s="5">
-        <v>3091.748</v>
+      <c r="N76" s="24">
+        <v>254530.54399999999</v>
+      </c>
+      <c r="O76">
+        <v>257254</v>
       </c>
       <c r="P76" s="5">
         <v>61.3</v>
@@ -5057,11 +5057,11 @@
       <c r="M77" s="5">
         <v>18068.599999999999</v>
       </c>
-      <c r="N77" s="5">
-        <v>3882.8989999999999</v>
-      </c>
-      <c r="O77" s="5">
-        <v>3091.748</v>
+      <c r="N77" s="24">
+        <v>257479.6586</v>
+      </c>
+      <c r="O77">
+        <v>261838</v>
       </c>
       <c r="P77" s="5">
         <v>69.7</v>
@@ -5110,11 +5110,11 @@
       <c r="M78" s="5">
         <v>17981.099999999999</v>
       </c>
-      <c r="N78" s="5">
-        <v>3966.989</v>
-      </c>
-      <c r="O78" s="5">
-        <v>3125.4209999999998</v>
+      <c r="N78" s="24">
+        <v>260110.71960000001</v>
+      </c>
+      <c r="O78">
+        <v>261796</v>
       </c>
       <c r="P78" s="5">
         <v>79</v>
@@ -5163,11 +5163,11 @@
       <c r="M79" s="5">
         <v>17882.099999999999</v>
       </c>
-      <c r="N79" s="5">
-        <v>3966.989</v>
-      </c>
-      <c r="O79" s="5">
-        <v>3125.4209999999998</v>
+      <c r="N79" s="24">
+        <v>265047.1778</v>
+      </c>
+      <c r="O79">
+        <v>269323</v>
       </c>
       <c r="P79" s="5">
         <v>76.900000000000006</v>
@@ -5216,11 +5216,11 @@
       <c r="M80" s="5">
         <v>18057.5</v>
       </c>
-      <c r="N80" s="5">
-        <v>3966.989</v>
-      </c>
-      <c r="O80" s="5">
-        <v>3125.4209999999998</v>
+      <c r="N80" s="24">
+        <v>262308.13020000001</v>
+      </c>
+      <c r="O80">
+        <v>265638</v>
       </c>
       <c r="P80" s="5">
         <v>79.400000000000006</v>
@@ -5269,11 +5269,11 @@
       <c r="M81" s="5">
         <v>18090</v>
       </c>
-      <c r="N81" s="5">
-        <v>4061.192</v>
-      </c>
-      <c r="O81" s="5">
-        <v>3154.3209999999999</v>
+      <c r="N81" s="24">
+        <v>269267.24300000002</v>
+      </c>
+      <c r="O81">
+        <v>266393</v>
       </c>
       <c r="P81" s="5">
         <v>77.2</v>
@@ -5322,11 +5322,11 @@
       <c r="M82" s="5">
         <v>17907</v>
       </c>
-      <c r="N82" s="5">
-        <v>4061.192</v>
-      </c>
-      <c r="O82" s="5">
-        <v>3154.3209999999999</v>
+      <c r="N82" s="24">
+        <v>268297.96049999999</v>
+      </c>
+      <c r="O82">
+        <v>264976</v>
       </c>
       <c r="P82" s="5">
         <v>69.099999999999994</v>
@@ -5375,11 +5375,11 @@
       <c r="M83" s="5">
         <v>18004.8</v>
       </c>
-      <c r="N83" s="5">
-        <v>4061.192</v>
-      </c>
-      <c r="O83" s="5">
-        <v>3154.3209999999999</v>
+      <c r="N83" s="24">
+        <v>270832.54519999999</v>
+      </c>
+      <c r="O83">
+        <v>268356</v>
       </c>
       <c r="P83" s="5">
         <v>68.2</v>
@@ -5428,11 +5428,11 @@
       <c r="M84" s="5">
         <v>17980.099999999999</v>
       </c>
-      <c r="N84" s="5">
-        <v>4163.9750000000004</v>
-      </c>
-      <c r="O84" s="5">
-        <v>3220.2919999999999</v>
+      <c r="N84" s="24">
+        <v>276766.47399999999</v>
+      </c>
+      <c r="O84">
+        <v>271115</v>
       </c>
       <c r="P84" s="5">
         <v>66.400000000000006</v>
@@ -5481,11 +5481,11 @@
       <c r="M85" s="5">
         <v>18046.599999999999</v>
       </c>
-      <c r="N85" s="5">
-        <v>4163.9750000000004</v>
-      </c>
-      <c r="O85" s="5">
-        <v>3220.2919999999999</v>
+      <c r="N85" s="24">
+        <v>272777.27720000001</v>
+      </c>
+      <c r="O85">
+        <v>275719</v>
       </c>
       <c r="P85" s="5">
         <v>67.900000000000006</v>
@@ -5534,11 +5534,11 @@
       <c r="M86" s="5">
         <v>18115.599999999999</v>
       </c>
-      <c r="N86" s="5">
-        <v>4163.9750000000004</v>
-      </c>
-      <c r="O86" s="5">
-        <v>3220.2919999999999</v>
+      <c r="N86" s="24">
+        <v>281009.27990000002</v>
+      </c>
+      <c r="O86">
+        <v>273687</v>
       </c>
       <c r="P86" s="5">
         <v>70.099999999999994</v>
@@ -5587,11 +5587,11 @@
       <c r="M87" s="5">
         <v>18150.8</v>
       </c>
-      <c r="N87" s="5">
-        <v>4141.0129999999999</v>
-      </c>
-      <c r="O87" s="5">
-        <v>3220.9290000000001</v>
+      <c r="N87" s="24">
+        <v>268698.69089999999</v>
+      </c>
+      <c r="O87">
+        <v>269501</v>
       </c>
       <c r="P87" s="5">
         <v>70.5</v>
@@ -5640,11 +5640,11 @@
       <c r="M88" s="5">
         <v>18325</v>
       </c>
-      <c r="N88" s="5">
-        <v>4141.0129999999999</v>
-      </c>
-      <c r="O88" s="5">
-        <v>3220.9290000000001</v>
+      <c r="N88" s="24">
+        <v>280404.36259999999</v>
+      </c>
+      <c r="O88">
+        <v>275828</v>
       </c>
       <c r="P88" s="5">
         <v>71.8</v>
@@ -5693,11 +5693,11 @@
       <c r="M89" s="5">
         <v>18500.2</v>
       </c>
-      <c r="N89" s="5">
-        <v>4141.0129999999999</v>
-      </c>
-      <c r="O89" s="5">
-        <v>3220.9290000000001</v>
+      <c r="N89" s="24">
+        <v>290890.33429999999</v>
+      </c>
+      <c r="O89">
+        <v>270192</v>
       </c>
       <c r="P89" s="5">
         <v>74</v>
@@ -5746,11 +5746,11 @@
       <c r="M90" s="5">
         <v>18473.2</v>
       </c>
-      <c r="N90" s="5">
-        <v>4548.8090000000002</v>
-      </c>
-      <c r="O90" s="5">
-        <v>3281.248</v>
+      <c r="N90" s="24">
+        <v>327795.77919999999</v>
+      </c>
+      <c r="O90">
+        <v>272436</v>
       </c>
       <c r="P90" s="5">
         <v>71.7</v>

</xml_diff>